<commit_message>
added APIServlet:getCourseListStudent(googleId) with tests
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Points calculation data.xlsx
+++ b/src/test/resources/data/Points calculation data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -117,8 +117,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,6 +280,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -358,6 +363,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -392,6 +398,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -567,14 +574,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="13"/>
     <col min="7" max="7" width="12.42578125" customWidth="1"/>
@@ -586,7 +593,7 @@
     <col min="23" max="23" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="13" customFormat="1">
+    <row r="1" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21"/>
       <c r="B1" s="21" t="s">
         <v>22</v>
@@ -621,7 +628,7 @@
       <c r="AA1" s="21"/>
       <c r="AB1" s="21"/>
     </row>
-    <row r="2" spans="1:28" s="13" customFormat="1">
+    <row r="2" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
@@ -694,7 +701,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
@@ -784,7 +791,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
@@ -874,7 +881,7 @@
         <v>299.99999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
@@ -964,7 +971,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
@@ -1054,7 +1061,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:28" s="13" customFormat="1">
+    <row r="9" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H9" s="22"/>
       <c r="I9" s="21" t="s">
         <v>26</v>
@@ -1068,7 +1075,7 @@
       <c r="P9" s="21"/>
       <c r="Q9" s="21"/>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="I10" s="15" t="s">
         <v>12</v>
       </c>
@@ -1095,7 +1102,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="I11" s="15" t="s">
         <v>13</v>
       </c>
@@ -1124,7 +1131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:28" s="25" customFormat="1" ht="30">
+    <row r="12" spans="1:28" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="H12" s="26"/>
       <c r="I12" s="28" t="s">
@@ -1147,7 +1154,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:28" hidden="1">
+    <row r="15" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="I15" s="15" t="s">
         <v>0</v>
       </c>
@@ -1173,7 +1180,7 @@
       </c>
       <c r="O15" s="23"/>
     </row>
-    <row r="16" spans="1:28" hidden="1">
+    <row r="16" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="I16" s="15" t="s">
         <v>1</v>
       </c>
@@ -1199,7 +1206,7 @@
       </c>
       <c r="O16" s="23"/>
     </row>
-    <row r="17" spans="1:18" hidden="1">
+    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="I17" s="15" t="s">
         <v>2</v>
       </c>
@@ -1225,7 +1232,7 @@
       </c>
       <c r="O17" s="23"/>
     </row>
-    <row r="18" spans="1:18" hidden="1">
+    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="I18" s="15" t="s">
         <v>3</v>
       </c>
@@ -1251,8 +1258,8 @@
       </c>
       <c r="O18" s="23"/>
     </row>
-    <row r="19" spans="1:18" hidden="1"/>
-    <row r="20" spans="1:18" s="25" customFormat="1" ht="69" hidden="1" customHeight="1">
+    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:18" s="25" customFormat="1" ht="69" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
       <c r="H20" s="26"/>
       <c r="I20" s="27" t="s">
@@ -1271,7 +1278,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:18" hidden="1">
+    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="I21" s="16" t="s">
         <v>15</v>
       </c>
@@ -1308,7 +1315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" hidden="1">
+    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="I22" s="16" t="s">
         <v>16</v>
       </c>
@@ -1345,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" hidden="1">
+    <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="I23" s="16" t="s">
         <v>17</v>
       </c>
@@ -1382,7 +1389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" hidden="1">
+    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="I24" s="16" t="s">
         <v>18</v>
       </c>
@@ -1419,8 +1426,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" hidden="1"/>
-    <row r="26" spans="1:18" ht="60">
+    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="I26" s="27" t="s">
         <v>30</v>
       </c>
@@ -1442,7 +1449,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I27" s="16" t="s">
         <v>15</v>
       </c>
@@ -1479,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I28" s="16" t="s">
         <v>16</v>
       </c>
@@ -1516,7 +1523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I29" s="16" t="s">
         <v>17</v>
       </c>
@@ -1553,7 +1560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I30" s="16" t="s">
         <v>18</v>
       </c>
@@ -1597,24 +1604,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>